<commit_message>
Add code to Tips 2 and 4
</commit_message>
<xml_diff>
--- a/ConsoleApp/TipsData.xlsx
+++ b/ConsoleApp/TipsData.xlsx
@@ -54,8 +54,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,32 +408,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:F7"/>
+  <dimension ref="C3:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C4" sqref="C4:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -438,7 +451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -452,7 +465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -466,7 +479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -482,8 +495,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <customProperties>
-    <customPr name="LastActive" r:id="rId1"/>
+    <customPr name="LastActive" r:id="rId2"/>
   </customProperties>
 </worksheet>
 </file>
</xml_diff>